<commit_message>
new barcodes, work in progress
</commit_message>
<xml_diff>
--- a/1-fastq_processing/index_list.xlsx
+++ b/1-fastq_processing/index_list.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krdav/Google Drive/MCB/Sullivan_lab/tRNA_charging/tRNAseq_pilot/seq_processing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krdav/Google Drive/MCB/Sullivan_lab/tRNA-charge-seq/1-fastq_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A192B0ED-CD9E-3D42-9D53-58E69B3E9DF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E1A1587-F88F-444C-9541-4DBB38255C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1960" yWindow="5960" windowWidth="26840" windowHeight="12040" xr2:uid="{74EA7424-48A6-C04A-A5DF-8688B5191606}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="58">
   <si>
     <t>type</t>
   </si>
@@ -136,13 +136,85 @@
   </si>
   <si>
     <t>CTTCGCCT</t>
+  </si>
+  <si>
+    <t>l1N</t>
+  </si>
+  <si>
+    <t>l2N</t>
+  </si>
+  <si>
+    <t>l3N</t>
+  </si>
+  <si>
+    <t>l4N</t>
+  </si>
+  <si>
+    <t>TNNNNNNGACTA</t>
+  </si>
+  <si>
+    <t>TNNNNNNAGTGC</t>
+  </si>
+  <si>
+    <t>TNNNNNNTCACG</t>
+  </si>
+  <si>
+    <t>TNNNNNNCTGAT</t>
+  </si>
+  <si>
+    <t>TNNNNNNGCATC</t>
+  </si>
+  <si>
+    <t>TNNNNNNAGCTG</t>
+  </si>
+  <si>
+    <t>TNNNNNNTAGCT</t>
+  </si>
+  <si>
+    <t>TNNNNNNTGCGA</t>
+  </si>
+  <si>
+    <t>TNNNNNNTACAG</t>
+  </si>
+  <si>
+    <t>TNNNNNNCATGA</t>
+  </si>
+  <si>
+    <t>TNNNNNNCTAGC</t>
+  </si>
+  <si>
+    <t>TNNNNNNGTACA</t>
+  </si>
+  <si>
+    <t>l5N</t>
+  </si>
+  <si>
+    <t>l6N</t>
+  </si>
+  <si>
+    <t>l7N</t>
+  </si>
+  <si>
+    <t>l8N</t>
+  </si>
+  <si>
+    <t>l9N</t>
+  </si>
+  <si>
+    <t>l10N</t>
+  </si>
+  <si>
+    <t>l11N</t>
+  </si>
+  <si>
+    <t>l12N</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -168,6 +240,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -189,10 +267,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,26 +586,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95D525E1-05CB-A24B-841E-93206D4958F2}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="188" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="188" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="15.83203125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -537,7 +619,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -548,7 +630,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -559,7 +641,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -570,7 +652,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -581,7 +663,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -592,7 +674,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -603,7 +685,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -614,7 +696,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -625,7 +707,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -636,61 +718,191 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>5</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="3" t="s">
         <v>20</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="3" t="s">
         <v>21</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="3" t="s">
         <v>22</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>5</v>
       </c>
       <c r="B15" t="s">
         <v>9</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>49</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>